<commit_message>
2nd revision of planning project
</commit_message>
<xml_diff>
--- a/Planificación del proyecto.xlsx
+++ b/Planificación del proyecto.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="81" uniqueCount="42">
   <si>
     <t>Semana 2</t>
   </si>
@@ -115,6 +115,33 @@
   </si>
   <si>
     <t>Design Website with dummy values and discuss the project</t>
+  </si>
+  <si>
+    <t>Tegshig</t>
+  </si>
+  <si>
+    <t>Tim</t>
+  </si>
+  <si>
+    <t>Start design of Node-Red</t>
+  </si>
+  <si>
+    <t>Luca</t>
+  </si>
+  <si>
+    <t>Finalize the website</t>
+  </si>
+  <si>
+    <t>Discuss the project</t>
+  </si>
+  <si>
+    <t>Optimizing website</t>
+  </si>
+  <si>
+    <t>Upload Project</t>
+  </si>
+  <si>
+    <t>K</t>
   </si>
 </sst>
 </file>
@@ -305,7 +332,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="20">
+  <cellXfs count="22">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
@@ -331,6 +358,22 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -339,18 +382,6 @@
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -657,17 +688,17 @@
   <dimension ref="A2:G72"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C26" sqref="C26"/>
+      <selection activeCell="B5" sqref="B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="53.28515625" customWidth="1"/>
     <col min="2" max="2" width="32.85546875" customWidth="1"/>
-    <col min="3" max="3" width="37.7109375" customWidth="1"/>
+    <col min="3" max="3" width="25.140625" customWidth="1"/>
     <col min="4" max="4" width="57.5703125" style="7" customWidth="1"/>
     <col min="5" max="5" width="38.28515625" customWidth="1"/>
-    <col min="6" max="6" width="47.28515625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="26" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
@@ -687,6 +718,9 @@
       <c r="A5" s="5" t="s">
         <v>13</v>
       </c>
+      <c r="B5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="10" t="s">
@@ -694,7 +728,7 @@
       </c>
       <c r="B6">
         <f>SUM(D:D)</f>
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="D6" s="9"/>
     </row>
@@ -704,59 +738,68 @@
       </c>
       <c r="B7">
         <f>SUM(G:G)</f>
-        <v>4.3</v>
+        <v>20.25</v>
       </c>
       <c r="D7" s="9"/>
     </row>
-    <row r="8" spans="1:7" ht="18" thickBot="1" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:7" ht="35.25" thickBot="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2"/>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="18" t="s">
         <v>15</v>
       </c>
       <c r="D8" s="8">
         <f>SUM(C10:C16)</f>
-        <v>0</v>
-      </c>
-      <c r="F8" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="F8" s="18" t="s">
         <v>15</v>
       </c>
       <c r="G8" s="8">
         <f>SUM(F10:F16)</f>
-        <v>2.15</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" s="19" customFormat="1" ht="34.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="16" t="s">
+        <v>6.75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" s="16" customFormat="1" ht="34.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="13" t="s">
         <v>16</v>
       </c>
-      <c r="B9" s="17" t="s">
+      <c r="B9" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="C9" s="18" t="s">
+      <c r="C9" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="D9" s="17" t="s">
+      <c r="D9" s="14" t="s">
         <v>21</v>
       </c>
-      <c r="E9" s="17" t="s">
+      <c r="E9" s="14" t="s">
         <v>22</v>
       </c>
-      <c r="F9" s="18" t="s">
+      <c r="F9" s="15" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>38</v>
+      </c>
+      <c r="B10" t="s">
+        <v>31</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
       <c r="D10" t="s">
         <v>19</v>
       </c>
       <c r="E10" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F10">
-        <v>1.1499999999999999</v>
+        <v>2.25</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -764,18 +807,29 @@
         <v>20</v>
       </c>
       <c r="E11" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D12" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="E12" t="s">
+        <v>34</v>
+      </c>
+      <c r="F12">
+        <v>2.25</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A19" s="13" t="s">
+      <c r="A19" s="19" t="s">
         <v>25</v>
       </c>
-      <c r="B19" s="14"/>
-      <c r="C19" s="15"/>
+      <c r="B19" s="20"/>
+      <c r="C19" s="21"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
@@ -808,7 +862,7 @@
       </c>
       <c r="G24" s="8">
         <f t="shared" ref="G24" si="1">SUM(F26:F32)</f>
-        <v>2.15</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -839,35 +893,55 @@
         <v>31</v>
       </c>
       <c r="C26">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D26" t="s">
         <v>24</v>
       </c>
       <c r="E26" t="s">
+        <v>33</v>
+      </c>
+      <c r="F26">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B27" t="s">
         <v>31</v>
       </c>
-      <c r="F26">
-        <v>1.1499999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="C27">
+        <v>1</v>
+      </c>
       <c r="D27" t="s">
         <v>23</v>
       </c>
       <c r="E27" t="s">
-        <v>31</v>
+        <v>36</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D28" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="E28" t="s">
+        <v>34</v>
+      </c>
+      <c r="F28">
+        <v>2.25</v>
       </c>
     </row>
     <row r="35" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A35" s="13" t="s">
+      <c r="A35" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B35" s="14"/>
-      <c r="C35" s="15"/>
+      <c r="B35" s="20"/>
+      <c r="C35" s="21"/>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
@@ -893,14 +967,14 @@
       </c>
       <c r="D40" s="8">
         <f t="shared" ref="D40" si="2">SUM(C42:C48)</f>
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="F40" s="2" t="s">
         <v>7</v>
       </c>
       <c r="G40" s="8">
         <f t="shared" ref="G40" si="3">SUM(F42:F48)</f>
-        <v>0</v>
+        <v>6.75</v>
       </c>
     </row>
     <row r="41" spans="1:7" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
@@ -923,12 +997,54 @@
         <v>6</v>
       </c>
     </row>
+    <row r="42" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A42" t="s">
+        <v>38</v>
+      </c>
+      <c r="B42" t="s">
+        <v>31</v>
+      </c>
+      <c r="C42">
+        <v>1</v>
+      </c>
+      <c r="D42" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="E42" s="17" t="s">
+        <v>33</v>
+      </c>
+      <c r="F42">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D43" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="E43" t="s">
+        <v>36</v>
+      </c>
+      <c r="F43">
+        <v>2.25</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="D44" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="E44" t="s">
+        <v>34</v>
+      </c>
+      <c r="F44">
+        <v>2.25</v>
+      </c>
+    </row>
     <row r="51" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A51" s="13" t="s">
+      <c r="A51" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B51" s="14"/>
-      <c r="C51" s="15"/>
+      <c r="B51" s="20"/>
+      <c r="C51" s="21"/>
     </row>
     <row r="55" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A55" s="11"/>
@@ -949,7 +1065,7 @@
       </c>
       <c r="D56" s="8">
         <f t="shared" ref="D56" si="4">SUM(C58:C64)</f>
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="F56" s="2" t="s">
         <v>7</v>
@@ -983,18 +1099,46 @@
       <c r="A58" t="s">
         <v>29</v>
       </c>
+      <c r="B58" t="s">
+        <v>31</v>
+      </c>
+      <c r="C58">
+        <v>1</v>
+      </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>30</v>
       </c>
+      <c r="B59" t="s">
+        <v>31</v>
+      </c>
+      <c r="C59">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" t="s">
+        <v>38</v>
+      </c>
+      <c r="B60" t="s">
+        <v>31</v>
+      </c>
+      <c r="C60">
+        <v>1</v>
+      </c>
     </row>
     <row r="67" spans="1:7" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A67" s="13" t="s">
+      <c r="A67" s="19" t="s">
         <v>9</v>
       </c>
-      <c r="B67" s="14"/>
-      <c r="C67" s="15"/>
+      <c r="B67" s="20"/>
+      <c r="C67" s="21"/>
+    </row>
+    <row r="68" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="B68" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="71" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A71" s="11"/>

</xml_diff>